<commit_message>
app install i18next plugin
</commit_message>
<xml_diff>
--- a/i18nTool/app.xlsx
+++ b/i18nTool/app.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>key</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -57,6 +57,78 @@
   </si>
   <si>
     <t>"測試"文件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>loginView.button.signIn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>loginView.desc.password</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>loginView.desc.loginID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>loginView.desc.plzSignIn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>login ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>登入名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>密码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>登入</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请登入帐户</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>密碼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>請登入帳戶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Password</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sign in</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Please sign in</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>loginView.desc.rememberMe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remember me</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>记住我</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>記住我</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -406,15 +478,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.875" customWidth="1"/>
+    <col min="1" max="1" width="32" customWidth="1"/>
     <col min="2" max="2" width="16.25" customWidth="1"/>
     <col min="3" max="3" width="16.75" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
@@ -436,33 +508,106 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A3:D8">
+    <sortCondition ref="A3"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>